<commit_message>
docs. update-um-tracking-template by YZ
</commit_message>
<xml_diff>
--- a/utm-tracking-template.xlsx
+++ b/utm-tracking-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5720" yWindow="1320" windowWidth="32200" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1320" windowWidth="28800" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="UMT 批量生成器" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="J18" sqref="J18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
docs. update MKG201 exercise-files
</commit_message>
<xml_diff>
--- a/utm-tracking-template.xlsx
+++ b/utm-tracking-template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>日期</t>
   </si>
@@ -119,7 +119,11 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>24-CNM12345678</t>
+    <t>yz-CNM12345678</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>yz-CNM12345678</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +545,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -682,7 +686,7 @@
       </c>
       <c r="R2" s="6" t="str">
         <f t="shared" ref="R2:R3" si="0">CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2)</f>
-        <v>http://mkg201demo.bpteach.com/?utm_source=zhihu.com&amp;utm_medium=referral&amp;utm_campaign=24-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
+        <v>http://mkg201demo.bpteach.com/?utm_source=zhihu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -717,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>4</v>
@@ -739,7 +743,7 @@
       </c>
       <c r="R3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>http://mkg201demo.bpteach.com/?utm_source=jianshu.com&amp;utm_medium=referral&amp;utm_campaign=24-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
+        <v>http://mkg201demo.bpteach.com/?utm_source=jianshu.com&amp;utm_medium=referral&amp;utm_campaign=yz-CNM12345678&amp;utm_term=7days-grow-up&amp;utm_content=textlink</v>
       </c>
     </row>
   </sheetData>

</xml_diff>